<commit_message>
Removed screws from *.MECH to top level BOM
</commit_message>
<xml_diff>
--- a/POSCON.MECH.BOM.xlsx
+++ b/POSCON.MECH.BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Product Name:</t>
   </si>
@@ -71,29 +71,6 @@
   </si>
   <si>
     <t>http://www.serpac.com/,  OEM Part No. RB221TC</t>
-  </si>
-  <si>
-    <t>Faceplate Mounting Screws</t>
-  </si>
-  <si>
-    <t>18-8 Stainless Steel Pan Head Phillips Machine Screw 4-40 thread, 9/16“ Length</t>
-  </si>
-  <si>
-    <t>91772A111</t>
-  </si>
-  <si>
-    <t>McMaster-Carr</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>http://www.mcmaster.com/#91772a111/=wy8q26</t>
-    </r>
   </si>
   <si>
     <t>Core Standoffs</t>
@@ -144,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -185,12 +162,6 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u val="single"/>
@@ -246,7 +217,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -271,22 +242,16 @@
     <xf numFmtId="14" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1543,18 +1508,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.7812" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5078" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7734" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="77.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.25" style="1" customWidth="1"/>
@@ -1683,7 +1648,7 @@
       <c r="H6" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1707,7 +1672,7 @@
     <row r="8" ht="16.5" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1747,7 +1712,7 @@
       <c r="D10" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="4"/>
       <c r="G10" t="s" s="5">
         <v>18</v>
@@ -1755,48 +1720,48 @@
       <c r="H10" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" ht="30.75" customHeight="1">
-      <c r="A11" s="4">
+    <row r="11" ht="16.5" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" ht="16.5" customHeight="1">
+      <c r="A12" s="5">
         <v>2</v>
       </c>
-      <c r="B11" t="s" s="6">
+      <c r="B12" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="C11" t="s" s="6">
+      <c r="C12" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="D11" t="s" s="6">
+      <c r="D12" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" t="s" s="6">
+      <c r="E12" s="9"/>
+      <c r="F12" s="4"/>
+      <c r="G12" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="H11" t="s" s="6">
+      <c r="H12" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1804,26 +1769,14 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="5">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s" s="5">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="E13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="4"/>
-      <c r="G13" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s" s="6">
-        <v>29</v>
-      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1831,14 +1784,26 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" ht="16.5" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="11"/>
+      <c r="A14" s="5">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E14" s="9"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="4"/>
+      <c r="G14" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s" s="6">
+        <v>29</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1846,29 +1811,17 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" ht="16.5" customHeight="1">
-      <c r="A15" s="5">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s" s="5">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="E15" s="10"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" t="s" s="5">
-        <v>33</v>
-      </c>
-      <c r="H15" t="s" s="6">
-        <v>34</v>
-      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
@@ -1876,7 +1829,9 @@
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" t="s" s="6">
+        <v>30</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1891,9 +1846,7 @@
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" t="s" s="6">
-        <v>35</v>
-      </c>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1906,9 +1859,9 @@
     </row>
     <row r="18" ht="16.5" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1921,9 +1874,9 @@
     </row>
     <row r="19" ht="16.5" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="9"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1936,62 +1889,62 @@
     </row>
     <row r="20" ht="16.5" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="4"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
     <row r="21" ht="16.5" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" ht="16.5" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="11"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
       <c r="M22" s="4"/>
     </row>
     <row r="23" ht="16.5" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
@@ -2030,34 +1983,18 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-    </row>
-    <row r="27" ht="16.5" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H11" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="H13" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="H12" r:id="rId1" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Minor edits - date and spelling
</commit_message>
<xml_diff>
--- a/POSCON.MECH.BOM.xlsx
+++ b/POSCON.MECH.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
     <t>Product Name:</t>
   </si>
   <si>
-    <t>Position Controller Mechanicals (VERSION 1.2 REV B)</t>
+    <t>Position Controller </t>
   </si>
   <si>
     <t>Tag:</t>
@@ -292,7 +292,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -364,7 +364,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>42131</v>
+        <v>42132</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>

</xml_diff>

<commit_message>
Added feedstocks to .MECH BOM
</commit_message>
<xml_diff>
--- a/POSCON.MECH.BOM.xlsx
+++ b/POSCON.MECH.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Product Name:</t>
   </si>
@@ -95,7 +95,7 @@
     <t>Backplate</t>
   </si>
   <si>
-    <t>1/8" Aluminum Plate with 4-40 threaded holes</t>
+    <t>Backing plate, 0.125” thick Aluminum with 4-40 threaded holes</t>
   </si>
   <si>
     <t>POSCON.BACK VER 1.2 REV C</t>
@@ -107,7 +107,22 @@
     <t>http://www.jmmfg.com/</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Delrin</t>
+  </si>
+  <si>
+    <t>Delrin (acetal resin), black, 0.125” thick</t>
+  </si>
+  <si>
     <t>     </t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>6061 Aluminum sheet, 0.125” thick</t>
   </si>
 </sst>
 </file>
@@ -289,10 +304,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -605,11 +620,17 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D16" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -621,6 +642,21 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H12" r:id="rId1" display="http://www.ponoko.com"/>

</xml_diff>